<commit_message>
Change ASKU in value set to asked-declined FHIR-41571 Migrate US Core Terminology to VSAC FHIR-42846,
</commit_message>
<xml_diff>
--- a/input/images/tables/assessments-valuesets.xlsx
+++ b/input/images/tables/assessments-valuesets.xlsx
@@ -478,7 +478,7 @@
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>Gravity</t>
+          <t>MCC</t>
         </is>
       </c>
     </row>
@@ -498,17 +498,17 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Social Determinants of Health Screening Assessments</t>
+          <t>Social Determinants of Health Screening Assessments and Questions</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1247.126/expansion</t>
+          <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1247.206/expansion</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2.16.840.1.113762.1.4.1247.126</t>
+          <t>2.16.840.1.113762.1.4.1247.206</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -523,7 +523,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -542,7 +542,7 @@
       <c r="A3" t="inlineStr"/>
       <c r="B3" t="inlineStr">
         <is>
-          <t>SDOH</t>
+          <t>!SDOH</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -552,17 +552,17 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>US Core SDOH Panel item Codes</t>
+          <t>Social Determinants of Health Screening Assessments</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>https://healthedata1.github.io/USCDI4-Sandbox/ValueSet-uscore-common-sdoh-assessments.html</t>
+          <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1247.126/expansion</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>2.16.840.1.113762.1.4.1247.126</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -572,15 +572,19 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>TRUE</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr"/>
+          <t>FALSE</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Set of SDOH Panel Codes</t>
+        </is>
+      </c>
       <c r="K3" t="inlineStr">
         <is>
           <t>TRUE</t>
@@ -592,7 +596,7 @@
       <c r="A4" t="inlineStr"/>
       <c r="B4" t="inlineStr">
         <is>
-          <t>SDOH</t>
+          <t>!SDOH</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -602,17 +606,17 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Caregiver Availability</t>
+          <t>US Core SDOH Panel item Codes</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1222.1058/expansion</t>
+          <t>https://healthedata1.github.io/USCDI4-Sandbox/ValueSet-uscore-common-sdoh-assessments.html</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2.16.840.1.113762.1.4.1222.1058</t>
+          <t>-</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -633,14 +637,10 @@
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr">
         <is>
-          <t>FALSE</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>TRUE</t>
-        </is>
-      </c>
+          <t>TRUE</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr"/>
@@ -656,17 +656,17 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Caregiver Characteristics</t>
+          <t>Caregiver Availability</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1222.1057/expansion</t>
+          <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1222.1058/expansion</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2.16.840.1.113762.1.4.1222.1057</t>
+          <t>2.16.840.1.113762.1.4.1222.1058</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -710,17 +710,17 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Criminal Justice Involvement or Incarceration History</t>
+          <t>Caregiver Characteristics</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1222.1082/expansion</t>
+          <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1222.1057/expansion</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2.16.840.1.113762.1.4.1222.1082</t>
+          <t>2.16.840.1.113762.1.4.1222.1057</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -764,17 +764,17 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Current or Former Occupation</t>
+          <t>Criminal Justice Involvement or Incarceration History</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1222.1048/expansion</t>
+          <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1222.1082/expansion</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2.16.840.1.113762.1.4.1222.1048</t>
+          <t>2.16.840.1.113762.1.4.1222.1082</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -818,17 +818,17 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Dependents in Home</t>
+          <t>Current or Former Occupation</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1222.1065/expansion</t>
+          <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1222.1048/expansion</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2.16.840.1.113762.1.4.1222.1065</t>
+          <t>2.16.840.1.113762.1.4.1222.1048</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -872,17 +872,17 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>English Proficiency</t>
+          <t>Dependents in Home</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1222.1030/expansion</t>
+          <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1222.1065/expansion</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2.16.840.1.113762.1.4.1222.1030</t>
+          <t>2.16.840.1.113762.1.4.1222.1065</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -926,17 +926,17 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Experiences of Discrimination</t>
+          <t>English Proficiency</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1222.1080/expansion</t>
+          <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1222.1030/expansion</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2.16.840.1.113762.1.4.1222.1080</t>
+          <t>2.16.840.1.113762.1.4.1222.1030</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -980,17 +980,17 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Exposure to Environmental Hazards</t>
+          <t>Experiences of Discrimination</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1222.1075/expansion</t>
+          <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1222.1080/expansion</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2.16.840.1.113762.1.4.1222.1075</t>
+          <t>2.16.840.1.113762.1.4.1222.1080</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -1034,17 +1034,17 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Immigration Status</t>
+          <t>Exposure to Environmental Hazards</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1222.1083/expansion</t>
+          <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1222.1075/expansion</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2.16.840.1.113762.1.4.1222.1083</t>
+          <t>2.16.840.1.113762.1.4.1222.1075</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -1088,17 +1088,17 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Income Level</t>
+          <t>Immigration Status</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1222.1053/expansion</t>
+          <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1222.1083/expansion</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2.16.840.1.113762.1.4.1222.1053</t>
+          <t>2.16.840.1.113762.1.4.1222.1083</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -1142,17 +1142,17 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Leisure Activity Engagement</t>
+          <t>Income Level</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1222.1069/expansion</t>
+          <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1222.1053/expansion</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2.16.840.1.113762.1.4.1222.1069</t>
+          <t>2.16.840.1.113762.1.4.1222.1053</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
@@ -1196,17 +1196,17 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Living Situation</t>
+          <t>Leisure Activity Engagement</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1222.1060/expansion</t>
+          <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1222.1069/expansion</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>2.16.840.1.113762.1.4.1222.1060</t>
+          <t>2.16.840.1.113762.1.4.1222.1069</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
@@ -1250,17 +1250,17 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Marital or Spousal Status</t>
+          <t>Living Situation</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1222.1064/expansion</t>
+          <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1222.1060/expansion</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>2.16.840.1.113762.1.4.1222.1064</t>
+          <t>2.16.840.1.113762.1.4.1222.1060</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -1304,17 +1304,17 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Neglect</t>
+          <t>Marital or Spousal Status</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1222.1042/expansion</t>
+          <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1222.1064/expansion</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>2.16.840.1.113762.1.4.1222.1042</t>
+          <t>2.16.840.1.113762.1.4.1222.1064</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
@@ -1358,17 +1358,17 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Physical Activity Level</t>
+          <t>Neglect</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1222.1068/expansion</t>
+          <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1222.1042/expansion</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>2.16.840.1.113762.1.4.1222.1068</t>
+          <t>2.16.840.1.113762.1.4.1222.1042</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
@@ -1412,17 +1412,17 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Unsafe Neighborhood</t>
+          <t>Physical Activity Level</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1222.1076/expansion</t>
+          <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1222.1068/expansion</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>2.16.840.1.113762.1.4.1222.1076</t>
+          <t>2.16.840.1.113762.1.4.1222.1068</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
@@ -1466,17 +1466,17 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Work Productivity</t>
+          <t>Unsafe Neighborhood</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1222.1050/expansion</t>
+          <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1222.1076/expansion</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>2.16.840.1.113762.1.4.1222.1050</t>
+          <t>2.16.840.1.113762.1.4.1222.1076</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
@@ -1507,32 +1507,30 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="n">
-        <v>2</v>
-      </c>
+      <c r="A21" t="inlineStr"/>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Functional Status</t>
+          <t>SDOH</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>functional-status</t>
+          <t>sdoh</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Functional Status Clinical Assessment</t>
+          <t>Work Productivity</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1222.1008/expansion</t>
+          <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1222.1050/expansion</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>2.16.840.1.113762.1.4.1222.1008</t>
+          <t>2.16.840.1.113762.1.4.1222.1050</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
@@ -1553,13 +1551,19 @@
       <c r="J21" t="inlineStr"/>
       <c r="K21" t="inlineStr">
         <is>
-          <t>TRUE</t>
-        </is>
-      </c>
-      <c r="L21" t="inlineStr"/>
+          <t>FALSE</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>TRUE</t>
+        </is>
+      </c>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr"/>
+      <c r="A22" t="n">
+        <v>2</v>
+      </c>
       <c r="B22" t="inlineStr">
         <is>
           <t>Functional Status</t>
@@ -1572,17 +1576,17 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Bathing or grooming/hygiene (ADL/IADL)</t>
+          <t>Functional Status Clinical Assessment</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1222.954/expansion</t>
+          <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1222.1008/expansion</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>2.16.840.1.113762.1.4.1222.954</t>
+          <t>2.16.840.1.113762.1.4.1222.1008</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
@@ -1603,7 +1607,7 @@
       <c r="J22" t="inlineStr"/>
       <c r="K22" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="L22" t="inlineStr"/>
@@ -1622,17 +1626,17 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Bed Mobility (ADL or IADL)</t>
+          <t>Bathing or grooming/hygiene (ADL/IADL)</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1222.962/expansion</t>
+          <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1222.954/expansion</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>2.16.840.1.113762.1.4.1222.962</t>
+          <t>2.16.840.1.113762.1.4.1222.954</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
@@ -1672,17 +1676,17 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Domestic Duties or Household Tasks (ADL/IADL)</t>
+          <t>Bed Mobility (ADL or IADL)</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1222.960/expansion</t>
+          <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1222.962/expansion</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>2.16.840.1.113762.1.4.1222.960</t>
+          <t>2.16.840.1.113762.1.4.1222.962</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
@@ -1722,17 +1726,17 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Dressing (ADL or IADL)</t>
+          <t>Domestic Duties or Household Tasks (ADL/IADL)</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1222.955/expansion</t>
+          <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1222.960/expansion</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>2.16.840.1.113762.1.4.1222.955</t>
+          <t>2.16.840.1.113762.1.4.1222.960</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
@@ -1772,17 +1776,17 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Fall Risk</t>
+          <t>Dressing (ADL or IADL)</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1222.711/expansion</t>
+          <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1222.955/expansion</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>2.16.840.1.113762.1.4.1222.711</t>
+          <t>2.16.840.1.113762.1.4.1222.955</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
@@ -1822,17 +1826,17 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Gait Quality</t>
+          <t>Fall Risk</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1222.826/expansion</t>
+          <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1222.711/expansion</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>2.16.840.1.113762.1.4.1222.826</t>
+          <t>2.16.840.1.113762.1.4.1222.711</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
@@ -1872,17 +1876,17 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Sit to Stand Ability</t>
+          <t>Gait Quality</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1222.836/expansion</t>
+          <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1222.826/expansion</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>2.16.840.1.113762.1.4.1222.836</t>
+          <t>2.16.840.1.113762.1.4.1222.826</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
@@ -1922,17 +1926,17 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Stair Use (ADL or IADL)</t>
+          <t>Sit to Stand Ability</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1222.963/expansion</t>
+          <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1222.836/expansion</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>2.16.840.1.113762.1.4.1222.963</t>
+          <t>2.16.840.1.113762.1.4.1222.836</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
@@ -1972,17 +1976,17 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Telephone Use (ADL or IADL)</t>
+          <t>Stair Use (ADL or IADL)</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1222.961/expansion</t>
+          <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1222.963/expansion</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>2.16.840.1.113762.1.4.1222.961</t>
+          <t>2.16.840.1.113762.1.4.1222.963</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
@@ -2022,17 +2026,17 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Toileting (ADL or IADL)</t>
+          <t>Telephone Use (ADL or IADL)</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1222.956/expansion</t>
+          <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1222.961/expansion</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>2.16.840.1.113762.1.4.1222.956</t>
+          <t>2.16.840.1.113762.1.4.1222.961</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
@@ -2072,17 +2076,17 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Transferring (ADL or IADL)</t>
+          <t>Toileting (ADL or IADL)</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1222.957/expansion</t>
+          <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1222.956/expansion</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>2.16.840.1.113762.1.4.1222.957</t>
+          <t>2.16.840.1.113762.1.4.1222.956</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
@@ -2122,17 +2126,17 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Walking or ambulation/locomotion (ADL/IADL)</t>
+          <t>Transferring (ADL or IADL)</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1222.958/expansion</t>
+          <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1222.957/expansion</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>2.16.840.1.113762.1.4.1222.958</t>
+          <t>2.16.840.1.113762.1.4.1222.957</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
@@ -2172,22 +2176,22 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Functional Status Clinician Interpretation</t>
+          <t>Walking or ambulation/locomotion (ADL/IADL)</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1222.1007/expansion</t>
+          <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1222.958/expansion</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>2.16.840.1.113762.1.4.1222.1007</t>
+          <t>2.16.840.1.113762.1.4.1222.958</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>TRUE</t>
+          <t>FALSE</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
@@ -2197,13 +2201,13 @@
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="J34" t="inlineStr"/>
       <c r="K34" t="inlineStr">
         <is>
-          <t>TRUE</t>
+          <t>FALSE</t>
         </is>
       </c>
       <c r="L34" t="inlineStr"/>
@@ -2212,7 +2216,7 @@
       <c r="A35" t="inlineStr"/>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Functional Status</t>
+          <t>!Functional Status</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -2222,27 +2226,27 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Functional Status Related Questionnaire Panel Codes</t>
+          <t>Functional Status Clinician Interpretation</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1222.1586/expansion</t>
+          <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1222.1007/expansion</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>2.16.840.1.113762.1.4.1222.1586</t>
+          <t>2.16.840.1.113762.1.4.1222.1007</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>TRUE</t>
+          <t>FALSE</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
@@ -2259,32 +2263,30 @@
       <c r="L35" t="inlineStr"/>
     </row>
     <row r="36">
-      <c r="A36" t="n">
-        <v>3</v>
-      </c>
+      <c r="A36" t="inlineStr"/>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Mental/Cognitive Status.</t>
+          <t>Functional Status</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>cognitive-status</t>
+          <t>functional-status</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Cognitive Health Related Questionnaire Panel Codes</t>
+          <t>Functional Status Related Questionnaire Panel Codes</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1222.1584/expansion</t>
+          <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1222.1586/expansion</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>2.16.840.1.113762.1.4.1222.1584</t>
+          <t>2.16.840.1.113762.1.4.1222.1586</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
@@ -2311,7 +2313,9 @@
       <c r="L36" t="inlineStr"/>
     </row>
     <row r="37">
-      <c r="A37" t="inlineStr"/>
+      <c r="A37" t="n">
+        <v>3</v>
+      </c>
       <c r="B37" t="inlineStr">
         <is>
           <t>Mental/Cognitive Status.</t>
@@ -2324,17 +2328,17 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Cognitive Function Clinical Assessment</t>
+          <t>Cognitive Health Related Questionnaire Panel Codes</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1222.981/expansion</t>
+          <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1222.1584/expansion</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>2.16.840.1.113762.1.4.1222.981</t>
+          <t>2.16.840.1.113762.1.4.1222.1584</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
@@ -2344,12 +2348,12 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>TRUE</t>
+          <t>FALSE</t>
         </is>
       </c>
       <c r="J37" t="inlineStr"/>
@@ -2374,22 +2378,22 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Cognitive Function Clinician Interpretation</t>
+          <t>Cognitive Function Clinical Assessment</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1222.979/expansion</t>
+          <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1222.981/expansion</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>2.16.840.1.113762.1.4.1222.979</t>
+          <t>2.16.840.1.113762.1.4.1222.981</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>TRUE</t>
+          <t>FALSE</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
@@ -2399,7 +2403,7 @@
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="J38" t="inlineStr"/>
@@ -2411,37 +2415,35 @@
       <c r="L38" t="inlineStr"/>
     </row>
     <row r="39">
-      <c r="A39" t="n">
-        <v>4</v>
-      </c>
+      <c r="A39" t="inlineStr"/>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Disability Status</t>
+          <t>Mental/Cognitive Status.</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>disability-status</t>
+          <t>cognitive-status</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Disability Status Assessment</t>
+          <t>Cognitive Function Clinician Interpretation</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1099.49/expansion</t>
+          <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1222.979/expansion</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>2.16.840.1.113762.1.4.1099.49</t>
+          <t>2.16.840.1.113762.1.4.1222.979</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
@@ -2451,7 +2453,7 @@
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>TRUE</t>
+          <t>FALSE</t>
         </is>
       </c>
       <c r="J39" t="inlineStr"/>
@@ -2464,31 +2466,31 @@
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Physical Activity</t>
+          <t>Disability Status</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>activity</t>
+          <t>disability-status</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>US Core PA Codes</t>
+          <t>Disability Status Assessment</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>https://healthedata1.github.io/USCDI4-Sandbox/ValueSet-uscore-pa-codes.html</t>
+          <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1099.49/expansion</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>2.16.840.1.113762.1.4.1099.49</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
@@ -2516,31 +2518,31 @@
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Alcohol Use</t>
+          <t>Physical Activity</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>social-history</t>
+          <t>activity</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Substance Use</t>
+          <t>US Core PA Codes</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1222.1015/expansion</t>
+          <t>https://healthedata1.github.io/USCDI4-Sandbox/ValueSet-uscore-pa-codes.html</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>2.16.840.1.113762.1.4.1222.1015</t>
+          <t>-</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
@@ -2567,7 +2569,9 @@
       <c r="L41" t="inlineStr"/>
     </row>
     <row r="42">
-      <c r="A42" t="inlineStr"/>
+      <c r="A42" t="n">
+        <v>6</v>
+      </c>
       <c r="B42" t="inlineStr">
         <is>
           <t>Alcohol Use</t>
@@ -2580,17 +2584,17 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Alcohol Use Related Questionnaire Panel Codes</t>
+          <t>Substance Use</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1222.1585/expansion</t>
+          <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1222.1015/expansion</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>2.16.840.1.113762.1.4.1222.1585</t>
+          <t>2.16.840.1.113762.1.4.1222.1015</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
@@ -2600,12 +2604,12 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>TRUE</t>
+          <t>FALSE</t>
         </is>
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="J42" t="inlineStr"/>
@@ -2617,12 +2621,10 @@
       <c r="L42" t="inlineStr"/>
     </row>
     <row r="43">
-      <c r="A43" t="n">
-        <v>7</v>
-      </c>
+      <c r="A43" t="inlineStr"/>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Substance Use</t>
+          <t>Alcohol Use</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -2632,17 +2634,17 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Substance Use</t>
+          <t>Alcohol Use Related Questionnaire Panel Codes</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1222.1015/expansion</t>
+          <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1222.1585/expansion</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>2.16.840.1.113762.1.4.1222.1015</t>
+          <t>2.16.840.1.113762.1.4.1222.1585</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
@@ -2652,12 +2654,12 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>TRUE</t>
+          <t>FALSE</t>
         </is>
       </c>
       <c r="J43" t="inlineStr"/>
@@ -2667,6 +2669,58 @@
         </is>
       </c>
       <c r="L43" t="inlineStr"/>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>7</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Substance Use</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>social-history</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Drug Misuse</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1222.707/expansion</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>2.16.840.1.113762.1.4.1222.707</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>FALSE</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>FALSE</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>TRUE</t>
+        </is>
+      </c>
+      <c r="J44" t="inlineStr"/>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>TRUE</t>
+        </is>
+      </c>
+      <c r="L44" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>

<commit_message>
remove Laboratory Report Narrative and Pathology Report Narrative from the USCDI table tracker pending??
</commit_message>
<xml_diff>
--- a/input/images/tables/assessments-valuesets.xlsx
+++ b/input/images/tables/assessments-valuesets.xlsx
@@ -2537,12 +2537,12 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>https://healthedata1.github.io/USCDI4-Sandbox/ValueSet-uscore-pa-codes.html</t>
+          <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1240.9/expansion</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>2.16.840.1.113762.1.4.1240.9</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">

</xml_diff>